<commit_message>
Otra vez Ale metió mano
</commit_message>
<xml_diff>
--- a/Resultados correlaciones.xlsx
+++ b/Resultados correlaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilo\Desktop\Apps\R Studio\Analisis articulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2608DB65-CB23-48B0-AC3A-EDF81FB0D404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F641099-8FDE-40F2-A074-C83ADB3F26C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D16CAE1A-F949-42E2-954C-BAFCBEFE2FD7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
   <si>
     <t xml:space="preserve">Amplificación </t>
   </si>
@@ -138,17 +138,131 @@
     <t xml:space="preserve">EDAD:CRI_Total </t>
   </si>
   <si>
-    <t xml:space="preserve">  0.03184 * </t>
-  </si>
-  <si>
     <t>MoCA:CRI_Total</t>
+  </si>
+  <si>
+    <t>value ~ EDAD * ESCOLARIDAD * MoCA * CRI_Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Intercept) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD </t>
+  </si>
+  <si>
+    <t>ESCOLARIDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRI_Total  </t>
+  </si>
+  <si>
+    <t>EDAD:ESCOLARIDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:MoCA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCOLARIDAD:MoCA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCOLARIDAD:CRI_Total  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoCA:CRI_Total   </t>
+  </si>
+  <si>
+    <t>EDAD:ESCOLARIDAD:MoCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:ESCOLARIDAD:CRI_Total   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:MoCA:CRI_Total  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCOLARIDAD:MoCA:CRI_Total    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:ESCOLARIDAD:MoCA:CRI_Total </t>
+  </si>
+  <si>
+    <t>value ~ EDAD + MoCA + CRI_Total + EDAD:MoCA + MoCA:CRI_Total</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoCA:CRI_Total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCOLARIDAD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoCA         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRI_Total   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:ESCOLARIDAD </t>
+  </si>
+  <si>
+    <t>ESCOLARIDAD:MoCA</t>
+  </si>
+  <si>
+    <t>EDAD:CRI_Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCOLARIDAD:CRI_Total    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoCA:CRI_Total           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:ESCOLARIDAD:MoCA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:ESCOLARIDAD:CRI_Total  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:MoCA:CRI_Total        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCOLARIDAD:MoCA:CRI_Total     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:ESCOLARIDAD:MoCA:CRI_Total  </t>
+  </si>
+  <si>
+    <t>ÍNDICE DE AMPLIFICACIÓN</t>
+  </si>
+  <si>
+    <t>value ~ ESCOLARIDAD + MoCA + ESCOLARIDAD:MoCA</t>
+  </si>
+  <si>
+    <t>value ~ EDAD + CRI_Total + EDAD:CRI_Total</t>
+  </si>
+  <si>
+    <t>ÍNDICES ATENCIONALES</t>
+  </si>
+  <si>
+    <t>ÍNDICE DE SUPRESIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCOLARIDAD:MoCA  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDAD:CRI_Total   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +279,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,19 +397,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,39 +770,39 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9" t="s">
+      <c r="J3" s="13"/>
+      <c r="K3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
@@ -683,10 +834,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -718,8 +869,8 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
@@ -749,8 +900,8 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -782,8 +933,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
@@ -813,10 +964,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -848,8 +999,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
@@ -879,8 +1030,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -912,8 +1063,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
@@ -943,11 +1094,11 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="5">
         <v>0.05</v>
       </c>
@@ -974,11 +1125,11 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="5">
         <v>-0.24</v>
       </c>
@@ -1005,11 +1156,11 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="5">
         <v>0.13</v>
       </c>
@@ -1036,11 +1187,11 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="5">
         <v>-0.19</v>
       </c>
@@ -1067,11 +1218,11 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="5">
         <v>0.05</v>
       </c>
@@ -1098,11 +1249,11 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="5">
         <v>0.09</v>
       </c>
@@ -1132,39 +1283,39 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9" t="s">
+      <c r="H21" s="13"/>
+      <c r="I21" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9" t="s">
+      <c r="J21" s="13"/>
+      <c r="K21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="9"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
@@ -1196,10 +1347,10 @@
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1231,8 +1382,8 @@
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1262,8 +1413,8 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1295,8 +1446,8 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="1" t="s">
         <v>3</v>
       </c>
@@ -1326,10 +1477,10 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1361,8 +1512,8 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
@@ -1392,8 +1543,8 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1425,8 +1576,8 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1456,11 +1607,11 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
       <c r="E31" s="8">
         <v>-0.14000000000000001</v>
       </c>
@@ -1487,11 +1638,11 @@
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
       <c r="E32" s="8">
         <v>0.36</v>
       </c>
@@ -1518,11 +1669,11 @@
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
       <c r="E33" s="8">
         <v>-0.22</v>
       </c>
@@ -1549,11 +1700,11 @@
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="8">
         <v>0.19</v>
       </c>
@@ -1580,11 +1731,11 @@
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="2">
         <v>-0.1</v>
       </c>
@@ -1611,11 +1762,11 @@
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="2">
         <v>-0.11</v>
       </c>
@@ -1687,177 +1838,1219 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E60CFDF-091D-4B15-A656-65BF75F7F5FE}">
-  <dimension ref="B2:K13"/>
+  <dimension ref="B2:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="61.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3">
+        <v>639.12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7.101</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.12839999999999999</v>
+      </c>
+      <c r="F5" s="12">
+        <v>3.8539999999999999E-6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3">
+        <v>516.77</v>
+      </c>
+      <c r="I5" s="3">
+        <v>5.6529999999999996</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.25209999999999999</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1.587E-9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="16">
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="16">
+        <v>7.1700000000000002E-3</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="16">
+        <v>-2.4089999999999998</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="16">
+        <v>1.694E-2</v>
+      </c>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="18">
+        <v>-1.385</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="18">
+        <v>0.16761999999999999</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="16">
+        <v>2.5259999999999998</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="16">
+        <v>1.235E-2</v>
+      </c>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="16">
+        <v>-2.294</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16">
+        <v>2.281E-2</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="16">
+        <v>3.0979999999999999</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="16">
+        <v>2.2399999999999998E-3</v>
+      </c>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16">
+        <v>-2.3319999999999999</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="16">
+        <v>2.0670000000000001E-2</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="16">
+        <v>2.33</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="16">
+        <v>2.087E-2</v>
+      </c>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="16">
+        <v>2.161</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="16">
+        <v>3.184E-2</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="18">
+        <v>1.8480000000000001</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="18">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="16">
+        <v>2.004</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16">
+        <v>4.6429999999999999E-2</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="16">
+        <v>-3.1819999999999999</v>
+      </c>
+      <c r="I12" s="17"/>
+      <c r="J12" s="16">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="16">
+        <v>-2.419</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="16">
+        <v>1.6490000000000001E-2</v>
+      </c>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="16">
+        <v>-2.9990000000000001</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="16">
+        <v>3.0699999999999998E-3</v>
+      </c>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="16">
+        <v>-1.9910000000000001</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="16">
+        <v>4.7849999999999997E-2</v>
+      </c>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="16">
+        <v>-2.532</v>
+      </c>
+      <c r="I16" s="17"/>
+      <c r="J16" s="16">
+        <v>1.214E-2</v>
+      </c>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="18">
+        <v>-1.7569999999999999</v>
+      </c>
+      <c r="I17" s="19"/>
+      <c r="J17" s="18">
+        <v>8.0560000000000007E-2</v>
+      </c>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="16">
+        <v>3.0670000000000002</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="J18" s="16">
+        <v>2.48E-3</v>
+      </c>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="16">
+        <v>2.677</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="16">
+        <v>8.0800000000000004E-3</v>
+      </c>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="18">
+        <v>1.8939999999999999</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="18">
+        <v>5.9790000000000003E-2</v>
+      </c>
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="16">
+        <v>2.4289999999999998</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="16">
+        <v>1.6049999999999998E-2</v>
+      </c>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="16">
+        <v>-2.5640000000000001</v>
+      </c>
+      <c r="I22" s="17"/>
+      <c r="J22" s="16">
+        <v>1.1129999999999999E-2</v>
+      </c>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E28" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
+      <c r="G28" s="10"/>
+      <c r="H28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J28" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K28" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2">
-        <v>639.12</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7.101</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.12839999999999999</v>
-      </c>
-      <c r="F5" s="13">
-        <v>3.8539999999999999E-6</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="3">
+        <v>-343.23</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5.9480000000000004</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="F29" s="12">
+        <v>3.7299999999999999E-5</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="3">
+        <v>-329.92</v>
+      </c>
+      <c r="I29" s="3">
+        <v>2.9119999999999999</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.1217</v>
+      </c>
+      <c r="K29" s="12">
+        <v>3.6049999999999998E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D30" s="22"/>
+      <c r="E30" s="20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="F30" s="22"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="J30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="18">
+        <v>-1.2609999999999999</v>
+      </c>
+      <c r="D31" s="19"/>
+      <c r="E31" s="18">
+        <v>0.20880000000000001</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8">
-        <v>2.7160000000000002</v>
-      </c>
-      <c r="D8">
-        <v>7.1700000000000002E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="H31" s="16">
+        <v>1.9730000000000001</v>
+      </c>
+      <c r="I31" s="17"/>
+      <c r="J31" s="16">
+        <v>4.99E-2</v>
+      </c>
+      <c r="K31" s="17"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9">
-        <v>-1.385</v>
-      </c>
-      <c r="D9">
-        <v>0.16761999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C32" s="18">
+        <v>-1.885</v>
+      </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="18">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="F32" s="19"/>
+      <c r="G32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="16">
+        <v>-2.1160000000000001</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="16">
+        <v>3.5650000000000001E-2</v>
+      </c>
+      <c r="K32" s="17"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10">
-        <v>-2.294</v>
-      </c>
-      <c r="D10">
-        <v>2.281E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11">
-        <v>-2.3319999999999999</v>
-      </c>
-      <c r="D11">
-        <v>2.0670000000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12">
-        <v>2.161</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13">
-        <v>2.004</v>
-      </c>
-      <c r="D13">
-        <v>4.6429999999999999E-2</v>
-      </c>
+      <c r="C33" s="18">
+        <v>1.921</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="18">
+        <v>5.6099999999999997E-2</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="16">
+        <v>-2.387</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="16">
+        <v>1.796E-2</v>
+      </c>
+      <c r="K33" s="17"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="16">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="16">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="18">
+        <v>-1.889</v>
+      </c>
+      <c r="I34" s="19"/>
+      <c r="J34" s="18">
+        <v>6.0440000000000001E-2</v>
+      </c>
+      <c r="K34" s="19"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="18">
+        <v>1.752</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="18">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="F35" s="19"/>
+      <c r="G35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" s="18">
+        <v>-1.502</v>
+      </c>
+      <c r="I35" s="19"/>
+      <c r="J35" s="18">
+        <v>0.13472000000000001</v>
+      </c>
+      <c r="K35" s="19"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="16">
+        <v>-1.9850000000000001</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="16">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="16">
+        <v>2.6030000000000002</v>
+      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="16">
+        <v>9.9799999999999993E-3</v>
+      </c>
+      <c r="K36" s="17"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="16">
+        <v>2.0430000000000001</v>
+      </c>
+      <c r="I37" s="17"/>
+      <c r="J37" s="16">
+        <v>4.2369999999999998E-2</v>
+      </c>
+      <c r="K37" s="17"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H38" s="16">
+        <v>2.3220000000000001</v>
+      </c>
+      <c r="I38" s="17"/>
+      <c r="J38" s="16">
+        <v>2.1309999999999999E-2</v>
+      </c>
+      <c r="K38" s="17"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H39" s="18">
+        <v>1.673</v>
+      </c>
+      <c r="I39" s="19"/>
+      <c r="J39" s="18">
+        <v>9.5869999999999997E-2</v>
+      </c>
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H40" s="18">
+        <v>1.909</v>
+      </c>
+      <c r="I40" s="19"/>
+      <c r="J40" s="18">
+        <v>5.7770000000000002E-2</v>
+      </c>
+      <c r="K40" s="19"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41" s="18">
+        <v>1.4390000000000001</v>
+      </c>
+      <c r="I41" s="19"/>
+      <c r="J41" s="18">
+        <v>0.15187</v>
+      </c>
+      <c r="K41" s="19"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H42" s="16">
+        <v>-2.516</v>
+      </c>
+      <c r="I42" s="17"/>
+      <c r="J42" s="16">
+        <v>1.269E-2</v>
+      </c>
+      <c r="K42" s="17"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" s="16">
+        <v>-2.129</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="16">
+        <v>3.4529999999999998E-2</v>
+      </c>
+      <c r="K43" s="17"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H44" s="18">
+        <v>-1.601</v>
+      </c>
+      <c r="I44" s="19"/>
+      <c r="J44" s="18">
+        <v>0.11094999999999999</v>
+      </c>
+      <c r="K44" s="19"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" s="18">
+        <v>-1.8380000000000001</v>
+      </c>
+      <c r="I45" s="19"/>
+      <c r="J45" s="18">
+        <v>6.7559999999999995E-2</v>
+      </c>
+      <c r="K45" s="19"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" s="16">
+        <v>2.0419999999999998</v>
+      </c>
+      <c r="I46" s="17"/>
+      <c r="J46" s="16">
+        <v>4.2569999999999997E-2</v>
+      </c>
+      <c r="K46" s="17"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+      <c r="C52" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K52" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="3">
+        <v>2471.94</v>
+      </c>
+      <c r="D53" s="3">
+        <v>3.6360000000000001</v>
+      </c>
+      <c r="E53" s="3">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1.376E-2</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H53" s="1">
+        <v>2518.52</v>
+      </c>
+      <c r="I53" s="1">
+        <v>2.4279999999999999</v>
+      </c>
+      <c r="J53" s="1">
+        <v>2.0279999999999999E-2</v>
+      </c>
+      <c r="K53" s="1">
+        <v>6.6540000000000002E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+      <c r="C54" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="15"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" s="15"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="13">
+        <v>1.9119999999999999</v>
+      </c>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13">
+        <v>5.7299999999999997E-2</v>
+      </c>
+      <c r="F55" s="13"/>
+      <c r="G55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H55" s="13">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="K55" s="13"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="14">
+        <v>-2.1219999999999999</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F56" s="14"/>
+      <c r="G56" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" s="13">
+        <v>-2.4380000000000002</v>
+      </c>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="K56" s="13"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="13">
+        <v>-1.966</v>
+      </c>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13">
+        <v>5.0599999999999999E-2</v>
+      </c>
+      <c r="F57" s="13"/>
+      <c r="G57" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H57" s="13">
+        <v>-1.8180000000000001</v>
+      </c>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13">
+        <v>7.0599999999999996E-2</v>
+      </c>
+      <c r="K57" s="13"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="14">
+        <v>2.2109999999999999</v>
+      </c>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14">
+        <v>2.81E-2</v>
+      </c>
+      <c r="F58" s="14"/>
+      <c r="G58" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H58" s="13">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13">
+        <v>2.98E-2</v>
+      </c>
+      <c r="K58" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="125">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="G51:K51"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B50:K50"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ya voy a subir los cambios porque por fin terminé. I'm free
</commit_message>
<xml_diff>
--- a/Resultados correlaciones.xlsx
+++ b/Resultados correlaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilo\Desktop\Apps\R Studio\Analisis articulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A958A26-613E-4E6F-B5A3-CEBCD08C8D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078D8DEF-8986-4F41-96AB-03B9663017FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D16CAE1A-F949-42E2-954C-BAFCBEFE2FD7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D16CAE1A-F949-42E2-954C-BAFCBEFE2FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="122">
   <si>
     <t xml:space="preserve">Amplificación </t>
   </si>
@@ -398,6 +398,12 @@
   </si>
   <si>
     <t>SUPRESION</t>
+  </si>
+  <si>
+    <t>Ignorar rostros</t>
+  </si>
+  <si>
+    <t>Atender rostros</t>
   </si>
 </sst>
 </file>
@@ -557,7 +563,34 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,19 +598,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -592,32 +622,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -934,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF383BE-99F2-400F-B9E5-02CFA7D3D216}">
-  <dimension ref="B2:L36"/>
+  <dimension ref="B2:V36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:L20"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,39 +957,39 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="16"/>
+      <c r="L3" s="24"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
@@ -1015,10 +1021,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1050,8 +1056,8 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1081,8 +1087,8 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1114,8 +1120,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1145,10 +1151,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1180,8 +1186,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1211,8 +1217,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1244,8 +1250,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1275,11 +1281,11 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="5">
         <v>0.05</v>
       </c>
@@ -1306,11 +1312,11 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="5">
         <v>-0.24</v>
       </c>
@@ -1337,11 +1343,11 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="5">
         <v>0.13</v>
       </c>
@@ -1368,11 +1374,11 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="5">
         <v>-0.19</v>
       </c>
@@ -1398,12 +1404,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B17" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="5">
         <v>0.05</v>
       </c>
@@ -1429,12 +1435,12 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="16" t="s">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="5">
         <v>0.09</v>
       </c>
@@ -1460,45 +1466,75 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16" t="s">
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16" t="s">
+      <c r="F21" s="24"/>
+      <c r="G21" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16" t="s">
+      <c r="H21" s="24"/>
+      <c r="I21" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16" t="s">
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="16"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L21" s="24"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="V21" s="24"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1526,12 +1562,37 @@
       <c r="L22" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="N22" s="1"/>
+      <c r="O22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B23" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1561,10 +1622,37 @@
       <c r="L23" s="2">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="N23" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="8">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="P23" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>-0.11</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="T23" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="V23" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1592,10 +1680,37 @@
       <c r="L24" s="2">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="16"/>
-      <c r="C25" s="16" t="s">
+      <c r="N24" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O24" s="2">
+        <v>-0.09</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>-0.11</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="S24" s="2">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="T24" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U24" s="2">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="V24" s="2">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1626,9 +1741,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="1" t="s">
         <v>3</v>
       </c>
@@ -1657,11 +1772,11 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B27" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1692,9 +1807,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
@@ -1723,9 +1838,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="16"/>
-      <c r="C29" s="16" t="s">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1755,10 +1870,21 @@
       <c r="L29" s="2">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1786,13 +1912,32 @@
       <c r="L30" s="2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="16" t="s">
+      <c r="N30" s="2"/>
+      <c r="O30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B31" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
       <c r="E31" s="8">
         <v>-0.14000000000000001</v>
       </c>
@@ -1817,13 +1962,34 @@
       <c r="L31" s="2">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="16" t="s">
+      <c r="N31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+      <c r="O31" s="1">
+        <v>-9.1259999999999994</v>
+      </c>
+      <c r="P31" s="1">
+        <v>-7.4371220000000002E-2</v>
+      </c>
+      <c r="Q31" s="37">
+        <v>2.2E-16</v>
+      </c>
+      <c r="R31" s="1">
+        <v>106.02</v>
+      </c>
+      <c r="S31" s="1">
+        <v>0.65482799999999997</v>
+      </c>
+      <c r="T31" s="36">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B32" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
       <c r="E32" s="8">
         <v>0.36</v>
       </c>
@@ -1850,11 +2016,11 @@
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="8">
         <v>-0.22</v>
       </c>
@@ -1881,11 +2047,11 @@
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="E34" s="8">
         <v>0.19</v>
       </c>
@@ -1912,11 +2078,11 @@
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="E35" s="2">
         <v>-0.1</v>
       </c>
@@ -1943,11 +2109,11 @@
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="E36" s="2">
         <v>-0.11</v>
       </c>
@@ -1974,7 +2140,39 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="44">
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="O29:Q29"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:C24"/>
@@ -1987,30 +2185,6 @@
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2021,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E60CFDF-091D-4B15-A656-65BF75F7F5FE}">
   <dimension ref="B2:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:K61"/>
+    <sheetView topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2040,34 +2214,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
@@ -2131,10 +2305,10 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="11" t="s">
         <v>27</v>
       </c>
@@ -2142,10 +2316,10 @@
         <v>16</v>
       </c>
       <c r="G6" s="10"/>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="11" t="s">
         <v>27</v>
       </c>
@@ -2157,10 +2331,10 @@
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="26">
         <v>156.99363600000001</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="13">
         <v>2.7160000000000002</v>
       </c>
@@ -2170,10 +2344,10 @@
       <c r="G7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="28">
         <v>-2394</v>
       </c>
-      <c r="I7" s="23"/>
+      <c r="I7" s="29"/>
       <c r="J7" s="13">
         <v>-2.4089999999999998</v>
       </c>
@@ -2185,10 +2359,10 @@
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="26">
         <v>-0.23292599999999999</v>
       </c>
-      <c r="D8" s="18"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="14">
         <v>-1.385</v>
       </c>
@@ -2198,70 +2372,70 @@
       <c r="G8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="28">
         <v>45.27</v>
       </c>
-      <c r="I8" s="23"/>
+      <c r="I8" s="29"/>
       <c r="J8" s="13">
         <v>2.5259999999999998</v>
       </c>
       <c r="K8" s="13">
         <v>1.235E-2</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="M8" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="N8" s="36" t="s">
+      <c r="N8" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="O8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="36" t="s">
+      <c r="P8" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="Q8" s="36" t="s">
+      <c r="Q8" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="36" t="s">
+      <c r="R8" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="28">
         <v>175.5</v>
       </c>
-      <c r="I9" s="23"/>
+      <c r="I9" s="29"/>
       <c r="J9" s="13">
         <v>3.0979999999999999</v>
       </c>
       <c r="K9" s="13">
         <v>2.2399999999999998E-3</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="M9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="36">
+      <c r="N9" s="22">
         <v>-0.23292599999999999</v>
       </c>
-      <c r="O9" s="36">
+      <c r="O9" s="22">
         <v>0.16761999999999999</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="Q9" s="37">
+      <c r="Q9" s="23">
         <v>45.27</v>
       </c>
-      <c r="R9" s="36">
+      <c r="R9" s="22">
         <v>1.235E-2</v>
       </c>
     </row>
@@ -2269,10 +2443,10 @@
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="26">
         <v>-4.5329969999999999</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="13">
         <v>-2.294</v>
       </c>
@@ -2282,28 +2456,28 @@
       <c r="G10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="28">
         <v>83.69</v>
       </c>
-      <c r="I10" s="23"/>
+      <c r="I10" s="29"/>
       <c r="J10" s="13">
         <v>2.33</v>
       </c>
       <c r="K10" s="13">
         <v>2.087E-2</v>
       </c>
-      <c r="M10" s="36" t="s">
+      <c r="M10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36" t="s">
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="Q10" s="37">
+      <c r="Q10" s="23">
         <v>175.5</v>
       </c>
-      <c r="R10" s="36">
+      <c r="R10" s="22">
         <v>2.2399999999999998E-3</v>
       </c>
     </row>
@@ -2311,10 +2485,10 @@
       <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="26">
         <v>-1.195784</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="13">
         <v>-2.3319999999999999</v>
       </c>
@@ -2324,131 +2498,131 @@
       <c r="G11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="28">
         <v>16.97</v>
       </c>
-      <c r="I11" s="23"/>
+      <c r="I11" s="29"/>
       <c r="J11" s="14">
         <v>1.8480000000000001</v>
       </c>
       <c r="K11" s="14">
         <v>6.6199999999999995E-2</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="M11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="22">
         <v>-4.5329969999999999</v>
       </c>
-      <c r="O11" s="36">
+      <c r="O11" s="22">
         <v>2.281E-2</v>
       </c>
-      <c r="P11" s="36" t="s">
+      <c r="P11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="23">
         <v>83.69</v>
       </c>
-      <c r="R11" s="36">
+      <c r="R11" s="22">
         <v>2.087E-2</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="28">
         <v>-3.2650000000000001</v>
       </c>
-      <c r="I12" s="23"/>
+      <c r="I12" s="29"/>
       <c r="J12" s="13">
         <v>-3.1819999999999999</v>
       </c>
       <c r="K12" s="13">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="M12" s="36" t="s">
+      <c r="M12" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="36">
+      <c r="N12" s="22">
         <v>-1.195784</v>
       </c>
-      <c r="O12" s="36">
+      <c r="O12" s="22">
         <v>2.0670000000000001E-2</v>
       </c>
-      <c r="P12" s="36" t="s">
+      <c r="P12" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="Q12" s="37">
+      <c r="Q12" s="23">
         <v>16.97</v>
       </c>
-      <c r="R12" s="36">
+      <c r="R12" s="22">
         <v>6.6199999999999995E-2</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="28">
         <v>-1.5720000000000001</v>
       </c>
-      <c r="I13" s="23"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="13">
         <v>-2.419</v>
       </c>
       <c r="K13" s="13">
         <v>1.6490000000000001E-2</v>
       </c>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="28">
         <v>-6.1589999999999998</v>
       </c>
-      <c r="I14" s="23"/>
+      <c r="I14" s="29"/>
       <c r="J14" s="13">
         <v>-2.9990000000000001</v>
       </c>
       <c r="K14" s="13">
         <v>3.0699999999999998E-3</v>
       </c>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="26">
         <v>3.3270000000000001E-3</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="13">
         <v>2.161</v>
       </c>
@@ -2458,70 +2632,70 @@
       <c r="G15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="28">
         <v>-0.32300000000000001</v>
       </c>
-      <c r="I15" s="23"/>
+      <c r="I15" s="29"/>
       <c r="J15" s="13">
         <v>-1.9910000000000001</v>
       </c>
       <c r="K15" s="13">
         <v>4.7849999999999997E-2</v>
       </c>
-      <c r="M15" s="36" t="s">
+      <c r="M15" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="N15" s="36" t="s">
+      <c r="N15" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="O15" s="36" t="s">
+      <c r="O15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="P15" s="36" t="s">
+      <c r="P15" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="Q15" s="36" t="s">
+      <c r="Q15" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="R15" s="36" t="s">
+      <c r="R15" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="28">
         <v>-1.2989999999999999</v>
       </c>
-      <c r="I16" s="23"/>
+      <c r="I16" s="29"/>
       <c r="J16" s="13">
         <v>-2.532</v>
       </c>
       <c r="K16" s="13">
         <v>1.214E-2</v>
       </c>
-      <c r="M16" s="36" t="s">
+      <c r="M16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N16" s="36">
+      <c r="N16" s="22">
         <v>-0.124</v>
       </c>
-      <c r="O16" s="36">
+      <c r="O16" s="22">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="P16" s="36" t="s">
+      <c r="P16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="36">
+      <c r="Q16" s="22">
         <v>-4.9550000000000001</v>
       </c>
-      <c r="R16" s="36">
+      <c r="R16" s="22">
         <v>3.5650000000000001E-2</v>
       </c>
     </row>
@@ -2529,10 +2703,10 @@
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="26">
         <v>3.4965000000000003E-2</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="13">
         <v>2.004</v>
       </c>
@@ -2542,120 +2716,120 @@
       <c r="G17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="28">
         <v>-0.58660000000000001</v>
       </c>
-      <c r="I17" s="23"/>
+      <c r="I17" s="29"/>
       <c r="J17" s="14">
         <v>-1.7569999999999999</v>
       </c>
       <c r="K17" s="14">
         <v>8.0560000000000007E-2</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="36">
+      <c r="N17" s="22">
         <v>0.11082599999999999</v>
       </c>
-      <c r="O17" s="36">
+      <c r="O17" s="22">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="P17" s="36" t="s">
+      <c r="P17" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="Q17" s="36">
+      <c r="Q17" s="22">
         <v>-1.8029999999999999</v>
       </c>
-      <c r="R17" s="36">
+      <c r="R17" s="22">
         <v>0.13472000000000001</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="32">
         <v>0.1144</v>
       </c>
-      <c r="I18" s="25"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="13">
         <v>3.0670000000000002</v>
       </c>
       <c r="K18" s="13">
         <v>2.48E-3</v>
       </c>
-      <c r="M18" s="36" t="s">
+      <c r="M18" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36" t="s">
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Q18" s="36">
+      <c r="Q18" s="22">
         <v>-17.670000000000002</v>
       </c>
-      <c r="R18" s="36">
+      <c r="R18" s="22">
         <v>1.796E-2</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="32">
         <v>2.4250000000000001E-2</v>
       </c>
-      <c r="I19" s="25"/>
+      <c r="I19" s="33"/>
       <c r="J19" s="13">
         <v>2.677</v>
       </c>
       <c r="K19" s="13">
         <v>8.0800000000000004E-3</v>
       </c>
-      <c r="M19" s="36" t="s">
+      <c r="M19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N19" s="36">
+      <c r="N19" s="22">
         <v>0.33983799999999997</v>
       </c>
-      <c r="O19" s="36">
+      <c r="O19" s="22">
         <v>5.6099999999999997E-2</v>
       </c>
-      <c r="P19" s="36" t="s">
+      <c r="P19" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="Q19" s="36">
+      <c r="Q19" s="22">
         <v>-8.8629999999999995</v>
       </c>
-      <c r="R19" s="36">
+      <c r="R19" s="22">
         <v>6.0440000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="32">
         <v>1.1180000000000001E-2</v>
       </c>
-      <c r="I20" s="25"/>
+      <c r="I20" s="33"/>
       <c r="J20" s="14">
         <v>1.8939999999999999</v>
       </c>
@@ -2665,17 +2839,17 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="32">
         <v>4.539E-2</v>
       </c>
-      <c r="I21" s="25"/>
+      <c r="I21" s="33"/>
       <c r="J21" s="13">
         <v>2.4289999999999998</v>
       </c>
@@ -2685,48 +2859,48 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="24">
+      <c r="H22" s="32">
         <v>-8.4780000000000001E-4</v>
       </c>
-      <c r="I22" s="25"/>
+      <c r="I22" s="33"/>
       <c r="J22" s="13">
         <v>-2.5640000000000001</v>
       </c>
       <c r="K22" s="13">
         <v>1.1129999999999999E-2</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="M22" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="N22" s="36" t="s">
+      <c r="N22" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="O22" s="36" t="s">
+      <c r="O22" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="P22" s="36" t="s">
+      <c r="P22" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="Q22" s="36" t="s">
+      <c r="Q22" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="R22" s="36" t="s">
+      <c r="R22" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="M23" s="36" t="s">
+      <c r="M23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36" t="s">
+      <c r="O23" s="22"/>
+      <c r="P23" s="22" t="s">
         <v>29</v>
       </c>
       <c r="Q23">
@@ -2737,11 +2911,11 @@
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="M24" s="36" t="s">
+      <c r="M24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36" t="s">
+      <c r="O24" s="22"/>
+      <c r="P24" s="22" t="s">
         <v>31</v>
       </c>
       <c r="Q24">
@@ -2752,7 +2926,7 @@
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="M25" s="36" t="s">
+      <c r="M25" s="22" t="s">
         <v>37</v>
       </c>
       <c r="N25">
@@ -2761,25 +2935,25 @@
       <c r="O25">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P25" s="36" t="s">
+      <c r="P25" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="R25" s="36"/>
+      <c r="R25" s="22"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="M26" s="36" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="M26" s="22" t="s">
         <v>30</v>
       </c>
       <c r="N26">
@@ -2788,27 +2962,27 @@
       <c r="O26">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="P26" s="36" t="s">
+      <c r="P26" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="R26" s="36"/>
+      <c r="R26" s="22"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21" t="s">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="R27" s="36"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="R27" s="22"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
@@ -2872,10 +3046,10 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="20"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="11" t="s">
         <v>27</v>
       </c>
@@ -2883,10 +3057,10 @@
         <v>16</v>
       </c>
       <c r="G30" s="10"/>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I30" s="20"/>
+      <c r="I30" s="31"/>
       <c r="J30" s="11" t="s">
         <v>27</v>
       </c>
@@ -2898,10 +3072,10 @@
       <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="26">
         <v>-6.0838190000000001</v>
       </c>
-      <c r="D31" s="18"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="14">
         <v>-1.2609999999999999</v>
       </c>
@@ -2911,10 +3085,10 @@
       <c r="G31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="28">
         <v>256.10000000000002</v>
       </c>
-      <c r="I31" s="23"/>
+      <c r="I31" s="29"/>
       <c r="J31" s="13">
         <v>1.9730000000000001</v>
       </c>
@@ -2926,10 +3100,10 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="26">
         <v>-0.124</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="14">
         <v>-1.885</v>
       </c>
@@ -2939,10 +3113,10 @@
       <c r="G32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H32" s="26">
         <v>-4.9550000000000001</v>
       </c>
-      <c r="I32" s="18"/>
+      <c r="I32" s="27"/>
       <c r="J32" s="13">
         <v>-2.1160000000000001</v>
       </c>
@@ -2952,17 +3126,17 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="28">
         <v>-17.670000000000002</v>
       </c>
-      <c r="I33" s="23"/>
+      <c r="I33" s="29"/>
       <c r="J33" s="13">
         <v>-2.387</v>
       </c>
@@ -2974,10 +3148,10 @@
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="26">
         <v>0.33983799999999997</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="14">
         <v>1.921</v>
       </c>
@@ -2987,10 +3161,10 @@
       <c r="G34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H34" s="26">
         <v>-8.8629999999999995</v>
       </c>
-      <c r="I34" s="18"/>
+      <c r="I34" s="27"/>
       <c r="J34" s="14">
         <v>-1.889</v>
       </c>
@@ -3002,10 +3176,10 @@
       <c r="B35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="26">
         <v>0.11082599999999999</v>
       </c>
-      <c r="D35" s="18"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="13">
         <v>2.0470000000000002</v>
       </c>
@@ -3015,10 +3189,10 @@
       <c r="G35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H35" s="17">
+      <c r="H35" s="26">
         <v>-1.8029999999999999</v>
       </c>
-      <c r="I35" s="18"/>
+      <c r="I35" s="27"/>
       <c r="J35" s="14">
         <v>-1.502</v>
       </c>
@@ -3028,17 +3202,17 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="22">
+      <c r="H36" s="28">
         <v>0.34889999999999999</v>
       </c>
-      <c r="I36" s="23"/>
+      <c r="I36" s="29"/>
       <c r="J36" s="13">
         <v>2.6030000000000002</v>
       </c>
@@ -3050,10 +3224,10 @@
       <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="26">
         <v>4.2290000000000001E-3</v>
       </c>
-      <c r="D37" s="18"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="14">
         <v>1.752</v>
       </c>
@@ -3063,10 +3237,10 @@
       <c r="G37" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H37" s="22">
+      <c r="H37" s="28">
         <v>0.17349999999999999</v>
       </c>
-      <c r="I37" s="23"/>
+      <c r="I37" s="29"/>
       <c r="J37" s="13">
         <v>2.0430000000000001</v>
       </c>
@@ -3076,17 +3250,17 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="3"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="22">
+      <c r="H38" s="28">
         <v>0.62290000000000001</v>
       </c>
-      <c r="I38" s="23"/>
+      <c r="I38" s="29"/>
       <c r="J38" s="13">
         <v>2.3220000000000001</v>
       </c>
@@ -3096,17 +3270,17 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="28">
         <v>3.5459999999999998E-2</v>
       </c>
-      <c r="I39" s="23"/>
+      <c r="I39" s="29"/>
       <c r="J39" s="14">
         <v>1.673</v>
       </c>
@@ -3116,17 +3290,17 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="22">
+      <c r="H40" s="28">
         <v>0.12790000000000001</v>
       </c>
-      <c r="I40" s="23"/>
+      <c r="I40" s="29"/>
       <c r="J40" s="14">
         <v>1.909</v>
       </c>
@@ -3138,10 +3312,10 @@
       <c r="B41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="26">
         <v>-3.9529999999999999E-3</v>
       </c>
-      <c r="D41" s="18"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="13">
         <v>-1.9850000000000001</v>
       </c>
@@ -3151,10 +3325,10 @@
       <c r="G41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H41" s="28">
         <v>6.275E-2</v>
       </c>
-      <c r="I41" s="23"/>
+      <c r="I41" s="29"/>
       <c r="J41" s="14">
         <v>1.4390000000000001</v>
       </c>
@@ -3164,17 +3338,17 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="3"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="G42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H42" s="28">
         <v>-1.226E-2</v>
       </c>
-      <c r="I42" s="23"/>
+      <c r="I42" s="29"/>
       <c r="J42" s="13">
         <v>-2.516</v>
       </c>
@@ -3184,17 +3358,17 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" s="3"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
       <c r="G43" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="22">
+      <c r="H43" s="28">
         <v>-2.5200000000000001E-3</v>
       </c>
-      <c r="I43" s="23"/>
+      <c r="I43" s="29"/>
       <c r="J43" s="13">
         <v>-2.129</v>
       </c>
@@ -3204,17 +3378,17 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="28">
         <v>-1.235E-3</v>
       </c>
-      <c r="I44" s="23"/>
+      <c r="I44" s="29"/>
       <c r="J44" s="14">
         <v>-1.601</v>
       </c>
@@ -3224,17 +3398,17 @@
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" s="3"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
       <c r="G45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="22">
+      <c r="H45" s="28">
         <v>-4.4869999999999997E-3</v>
       </c>
-      <c r="I45" s="23"/>
+      <c r="I45" s="29"/>
       <c r="J45" s="14">
         <v>-1.8380000000000001</v>
       </c>
@@ -3244,17 +3418,17 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" s="3"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
       <c r="G46" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H46" s="22">
+      <c r="H46" s="28">
         <v>8.8200000000000003E-5</v>
       </c>
-      <c r="I46" s="23"/>
+      <c r="I46" s="29"/>
       <c r="J46" s="13">
         <v>2.0419999999999998</v>
       </c>
@@ -3263,34 +3437,34 @@
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="30"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21" t="s">
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
@@ -3354,10 +3528,10 @@
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D54" s="20"/>
+      <c r="D54" s="31"/>
       <c r="E54" s="11" t="s">
         <v>27</v>
       </c>
@@ -3365,10 +3539,10 @@
         <v>16</v>
       </c>
       <c r="G54" s="1"/>
-      <c r="H54" s="20" t="s">
+      <c r="H54" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I54" s="20"/>
+      <c r="I54" s="31"/>
       <c r="J54" s="11" t="s">
         <v>27</v>
       </c>
@@ -3380,10 +3554,10 @@
       <c r="B55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="17">
+      <c r="C55" s="26">
         <v>6656.6639999999998</v>
       </c>
-      <c r="D55" s="18"/>
+      <c r="D55" s="27"/>
       <c r="E55" s="14">
         <v>1.9119999999999999</v>
       </c>
@@ -3393,10 +3567,10 @@
       <c r="G55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H55" s="17">
+      <c r="H55" s="26">
         <v>1673.6934000000001</v>
       </c>
-      <c r="I55" s="18"/>
+      <c r="I55" s="27"/>
       <c r="J55" s="14">
         <v>2.2320000000000002</v>
       </c>
@@ -3406,17 +3580,17 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" s="3"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="18"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="27"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H56" s="17">
+      <c r="H56" s="26">
         <v>-34.612099999999998</v>
       </c>
-      <c r="I56" s="18"/>
+      <c r="I56" s="27"/>
       <c r="J56" s="14">
         <v>-2.4380000000000002</v>
       </c>
@@ -3428,10 +3602,10 @@
       <c r="B57" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="17">
+      <c r="C57" s="26">
         <v>-423.01299999999998</v>
       </c>
-      <c r="D57" s="18"/>
+      <c r="D57" s="27"/>
       <c r="E57" s="13">
         <v>-2.1219999999999999</v>
       </c>
@@ -3439,8 +3613,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="18"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="27"/>
       <c r="J57" s="14"/>
       <c r="K57" s="14"/>
     </row>
@@ -3448,10 +3622,10 @@
       <c r="B58" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="17">
+      <c r="C58" s="26">
         <v>-251.28800000000001</v>
       </c>
-      <c r="D58" s="18"/>
+      <c r="D58" s="27"/>
       <c r="E58" s="14">
         <v>-1.966</v>
       </c>
@@ -3459,24 +3633,24 @@
         <v>5.0599999999999999E-2</v>
       </c>
       <c r="G58" s="1"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="18"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="27"/>
       <c r="J58" s="14"/>
       <c r="K58" s="14"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" s="3"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="18"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="27"/>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H59" s="17">
+      <c r="H59" s="26">
         <v>-13.111700000000001</v>
       </c>
-      <c r="I59" s="18"/>
+      <c r="I59" s="27"/>
       <c r="J59" s="14">
         <v>-1.8180000000000001</v>
       </c>
@@ -3488,10 +3662,10 @@
       <c r="B60" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="17">
+      <c r="C60" s="26">
         <v>16.175000000000001</v>
       </c>
-      <c r="D60" s="18"/>
+      <c r="D60" s="27"/>
       <c r="E60" s="13">
         <v>2.2109999999999999</v>
       </c>
@@ -3499,24 +3673,24 @@
         <v>2.81E-2</v>
       </c>
       <c r="G60" s="1"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="18"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="27"/>
       <c r="J60" s="14"/>
       <c r="K60" s="14"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
       <c r="G61" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H61" s="17">
+      <c r="H61" s="26">
         <v>0.28439999999999999</v>
       </c>
-      <c r="I61" s="18"/>
+      <c r="I61" s="27"/>
       <c r="J61" s="14">
         <v>2.1880000000000002</v>
       </c>
@@ -3526,11 +3700,67 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B50:K50"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="G51:K51"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="H6:I6"/>
@@ -3539,7 +3769,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C16:D16"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C12:D12"/>
@@ -3548,6 +3777,12 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H16:I16"/>
@@ -3558,67 +3793,6 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="G51:K51"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B50:K50"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3640,12 +3814,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3654,14 +3828,14 @@
       <c r="K2" s="12"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -3769,22 +3943,22 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="26" t="s">
+      <c r="C19" s="30"/>
+      <c r="D19" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="27"/>
+      <c r="E19" s="35"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
@@ -3807,198 +3981,198 @@
       <c r="C21" s="8">
         <v>2471.94</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="18">
         <v>2518.52</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="2">
         <v>2473.62</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="19">
         <v>2520.5</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="2">
         <v>2474.63</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="19">
         <v>2520.98</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="2">
         <v>2475.84</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="19">
         <v>2522.96</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="2">
         <v>2477.54</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="19">
         <v>2523.08</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="2">
         <v>2479.5</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="20">
         <v>2524.15</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="2">
         <v>2480.9899999999998</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="19">
         <v>2525.4699999999998</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="2">
         <v>2482.6</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="19">
         <v>2527.2199999999998</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="2">
         <v>2484.46</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="19">
         <v>2528.56</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="2">
         <v>2486.02</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="33">
+      <c r="E30" s="19">
         <v>2529.6</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="2">
         <v>2487.36</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="33">
+      <c r="E31" s="19">
         <v>2529.85</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="2">
         <v>2489.3000000000002</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="19">
         <v>2531.27</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="28">
+      <c r="C33" s="2">
         <v>2489.4899999999998</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="21">
         <v>2533.0500000000002</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="26" t="s">
+      <c r="C38" s="30"/>
+      <c r="D38" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="27"/>
+      <c r="E38" s="35"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
@@ -4015,130 +4189,130 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="31">
+      <c r="C40" s="17">
         <v>-333.08</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E40" s="31">
+      <c r="E40" s="17">
         <v>-329.92</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="30">
+      <c r="C41" s="15">
         <v>-335.08</v>
       </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="30">
+      <c r="C42" s="15">
         <v>-337</v>
       </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C43" s="30">
+      <c r="C43" s="15">
         <v>-338.25</v>
       </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="30">
+      <c r="C44" s="15">
         <v>-340.16</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="30">
+      <c r="C45" s="15">
         <v>-340.51</v>
       </c>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="30">
+      <c r="C46" s="15">
         <v>-341.61</v>
       </c>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="30">
+      <c r="C47" s="15">
         <v>-341.65</v>
       </c>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="30">
+      <c r="C48" s="15">
         <v>-342.27</v>
       </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="30">
+      <c r="C49" s="15">
         <v>-342.61</v>
       </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="30">
+      <c r="C50" s="15">
         <v>-343.23</v>
       </c>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cambios con el nuevo EI
</commit_message>
<xml_diff>
--- a/Resultados correlaciones.xlsx
+++ b/Resultados correlaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilo\Desktop\Apps\R Studio\Analisis articulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078D8DEF-8986-4F41-96AB-03B9663017FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BBB6A9-211C-434D-AA28-9334FA39B2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D16CAE1A-F949-42E2-954C-BAFCBEFE2FD7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="123">
   <si>
     <t xml:space="preserve">Amplificación </t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t>Atender rostros</t>
+  </si>
+  <si>
+    <t>EI NUEVO CON D PRIMA</t>
   </si>
 </sst>
 </file>
@@ -455,7 +458,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -515,11 +518,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -586,11 +600,15 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -598,16 +616,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -622,8 +640,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -940,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF383BE-99F2-400F-B9E5-02CFA7D3D216}">
-  <dimension ref="B2:V36"/>
+  <dimension ref="B2:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29:T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -957,39 +980,39 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24" t="s">
+      <c r="J3" s="27"/>
+      <c r="K3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="24"/>
+      <c r="L3" s="27"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
@@ -1021,10 +1044,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="27" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1056,8 +1079,8 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1087,8 +1110,8 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="24"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1120,8 +1143,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1151,10 +1174,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="27" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1186,8 +1209,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1217,8 +1240,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="27" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1250,8 +1273,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1281,11 +1304,11 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="5">
         <v>0.05</v>
       </c>
@@ -1312,11 +1335,11 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="5">
         <v>-0.24</v>
       </c>
@@ -1343,11 +1366,11 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="5">
         <v>0.13</v>
       </c>
@@ -1374,11 +1397,11 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="5">
         <v>-0.19</v>
       </c>
@@ -1404,12 +1427,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B17" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="5">
         <v>0.05</v>
       </c>
@@ -1435,12 +1458,12 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B18" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="5">
         <v>0.09</v>
       </c>
@@ -1466,75 +1489,89 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24" t="s">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="24" t="s">
+      <c r="O20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24" t="s">
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="39"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24" t="s">
+      <c r="F21" s="27"/>
+      <c r="G21" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24" t="s">
+      <c r="H21" s="27"/>
+      <c r="I21" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24" t="s">
+      <c r="J21" s="27"/>
+      <c r="K21" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="L21" s="24"/>
+      <c r="L21" s="27"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="24" t="s">
+      <c r="O21" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24" t="s">
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24" t="s">
+      <c r="R21" s="27"/>
+      <c r="S21" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24" t="s">
+      <c r="T21" s="27"/>
+      <c r="U21" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="V21" s="24"/>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="V21" s="27"/>
+      <c r="W21" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z21" s="39"/>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1587,12 +1624,24 @@
       <c r="V22" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B23" s="24" t="s">
+      <c r="W22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B23" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="27" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1649,10 +1698,22 @@
       <c r="V23" s="2">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="W23" s="2">
+        <v>-0.11</v>
+      </c>
+      <c r="X23" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1707,10 +1768,22 @@
       <c r="V24" s="2">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B25" s="24"/>
-      <c r="C25" s="24" t="s">
+      <c r="W24" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="X24" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="Z24" s="2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="25" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B25" s="27"/>
+      <c r="C25" s="27" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1741,9 +1814,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+    <row r="26" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="1" t="s">
         <v>3</v>
       </c>
@@ -1772,11 +1845,11 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B27" s="24" t="s">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B27" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="27" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1807,9 +1880,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
@@ -1838,9 +1911,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B29" s="24"/>
-      <c r="C29" s="24" t="s">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B29" s="27"/>
+      <c r="C29" s="27" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1871,20 +1944,20 @@
         <v>0.7</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="O29" s="25" t="s">
+      <c r="O29" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25" t="s">
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-    </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+    </row>
+    <row r="30" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1932,12 +2005,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="s">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B31" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="8">
         <v>-0.14000000000000001</v>
       </c>
@@ -1971,7 +2044,7 @@
       <c r="P31" s="1">
         <v>-7.4371220000000002E-2</v>
       </c>
-      <c r="Q31" s="37">
+      <c r="Q31" s="25">
         <v>2.2E-16</v>
       </c>
       <c r="R31" s="1">
@@ -1980,16 +2053,16 @@
       <c r="S31" s="1">
         <v>0.65482799999999997</v>
       </c>
-      <c r="T31" s="36">
+      <c r="T31" s="24">
         <v>2.2E-16</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B32" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="8">
         <v>0.36</v>
       </c>
@@ -2016,11 +2089,11 @@
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="8">
         <v>-0.22</v>
       </c>
@@ -2047,11 +2120,11 @@
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="8">
         <v>0.19</v>
       </c>
@@ -2078,11 +2151,11 @@
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="2">
         <v>-0.1</v>
       </c>
@@ -2109,11 +2182,11 @@
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="2">
         <v>-0.11</v>
       </c>
@@ -2140,27 +2213,22 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:D14"/>
+  <mergeCells count="47">
+    <mergeCell ref="W20:Z20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="I21:J21"/>
@@ -2173,18 +2241,26 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="O29:Q29"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2331,10 +2407,10 @@
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="28">
         <v>156.99363600000001</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="13">
         <v>2.7160000000000002</v>
       </c>
@@ -2344,10 +2420,10 @@
       <c r="G7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="32">
         <v>-2394</v>
       </c>
-      <c r="I7" s="29"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="13">
         <v>-2.4089999999999998</v>
       </c>
@@ -2359,10 +2435,10 @@
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="28">
         <v>-0.23292599999999999</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="14">
         <v>-1.385</v>
       </c>
@@ -2372,10 +2448,10 @@
       <c r="G8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="32">
         <v>45.27</v>
       </c>
-      <c r="I8" s="29"/>
+      <c r="I8" s="33"/>
       <c r="J8" s="13">
         <v>2.5259999999999998</v>
       </c>
@@ -2403,17 +2479,17 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="32">
         <v>175.5</v>
       </c>
-      <c r="I9" s="29"/>
+      <c r="I9" s="33"/>
       <c r="J9" s="13">
         <v>3.0979999999999999</v>
       </c>
@@ -2443,10 +2519,10 @@
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="28">
         <v>-4.5329969999999999</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="13">
         <v>-2.294</v>
       </c>
@@ -2456,10 +2532,10 @@
       <c r="G10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="32">
         <v>83.69</v>
       </c>
-      <c r="I10" s="29"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="13">
         <v>2.33</v>
       </c>
@@ -2485,10 +2561,10 @@
       <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="28">
         <v>-1.195784</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="13">
         <v>-2.3319999999999999</v>
       </c>
@@ -2498,10 +2574,10 @@
       <c r="G11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="32">
         <v>16.97</v>
       </c>
-      <c r="I11" s="29"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="14">
         <v>1.8480000000000001</v>
       </c>
@@ -2529,17 +2605,17 @@
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="32">
         <v>-3.2650000000000001</v>
       </c>
-      <c r="I12" s="29"/>
+      <c r="I12" s="33"/>
       <c r="J12" s="13">
         <v>-3.1819999999999999</v>
       </c>
@@ -2567,17 +2643,17 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="32">
         <v>-1.5720000000000001</v>
       </c>
-      <c r="I13" s="29"/>
+      <c r="I13" s="33"/>
       <c r="J13" s="13">
         <v>-2.419</v>
       </c>
@@ -2593,17 +2669,17 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="32">
         <v>-6.1589999999999998</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="33"/>
       <c r="J14" s="13">
         <v>-2.9990000000000001</v>
       </c>
@@ -2619,10 +2695,10 @@
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="28">
         <v>3.3270000000000001E-3</v>
       </c>
-      <c r="D15" s="27"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="13">
         <v>2.161</v>
       </c>
@@ -2632,10 +2708,10 @@
       <c r="G15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="32">
         <v>-0.32300000000000001</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="33"/>
       <c r="J15" s="13">
         <v>-1.9910000000000001</v>
       </c>
@@ -2663,17 +2739,17 @@
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="32">
         <v>-1.2989999999999999</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="13">
         <v>-2.532</v>
       </c>
@@ -2703,10 +2779,10 @@
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="28">
         <v>3.4965000000000003E-2</v>
       </c>
-      <c r="D17" s="27"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="13">
         <v>2.004</v>
       </c>
@@ -2716,10 +2792,10 @@
       <c r="G17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="32">
         <v>-0.58660000000000001</v>
       </c>
-      <c r="I17" s="29"/>
+      <c r="I17" s="33"/>
       <c r="J17" s="14">
         <v>-1.7569999999999999</v>
       </c>
@@ -2747,17 +2823,17 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="34">
         <v>0.1144</v>
       </c>
-      <c r="I18" s="33"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="13">
         <v>3.0670000000000002</v>
       </c>
@@ -2781,17 +2857,17 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="34">
         <v>2.4250000000000001E-2</v>
       </c>
-      <c r="I19" s="33"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="13">
         <v>2.677</v>
       </c>
@@ -2819,17 +2895,17 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="34">
         <v>1.1180000000000001E-2</v>
       </c>
-      <c r="I20" s="33"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="14">
         <v>1.8939999999999999</v>
       </c>
@@ -2839,17 +2915,17 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="34">
         <v>4.539E-2</v>
       </c>
-      <c r="I21" s="33"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="13">
         <v>2.4289999999999998</v>
       </c>
@@ -2859,17 +2935,17 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="34">
         <v>-8.4780000000000001E-4</v>
       </c>
-      <c r="I22" s="33"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="13">
         <v>-2.5640000000000001</v>
       </c>
@@ -3072,10 +3148,10 @@
       <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="28">
         <v>-6.0838190000000001</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="14">
         <v>-1.2609999999999999</v>
       </c>
@@ -3085,10 +3161,10 @@
       <c r="G31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="28">
+      <c r="H31" s="32">
         <v>256.10000000000002</v>
       </c>
-      <c r="I31" s="29"/>
+      <c r="I31" s="33"/>
       <c r="J31" s="13">
         <v>1.9730000000000001</v>
       </c>
@@ -3100,10 +3176,10 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="28">
         <v>-0.124</v>
       </c>
-      <c r="D32" s="27"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="14">
         <v>-1.885</v>
       </c>
@@ -3113,10 +3189,10 @@
       <c r="G32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="26">
+      <c r="H32" s="28">
         <v>-4.9550000000000001</v>
       </c>
-      <c r="I32" s="27"/>
+      <c r="I32" s="29"/>
       <c r="J32" s="13">
         <v>-2.1160000000000001</v>
       </c>
@@ -3126,17 +3202,17 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="28">
+      <c r="H33" s="32">
         <v>-17.670000000000002</v>
       </c>
-      <c r="I33" s="29"/>
+      <c r="I33" s="33"/>
       <c r="J33" s="13">
         <v>-2.387</v>
       </c>
@@ -3148,10 +3224,10 @@
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="28">
         <v>0.33983799999999997</v>
       </c>
-      <c r="D34" s="27"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="14">
         <v>1.921</v>
       </c>
@@ -3161,10 +3237,10 @@
       <c r="G34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H34" s="26">
+      <c r="H34" s="28">
         <v>-8.8629999999999995</v>
       </c>
-      <c r="I34" s="27"/>
+      <c r="I34" s="29"/>
       <c r="J34" s="14">
         <v>-1.889</v>
       </c>
@@ -3176,10 +3252,10 @@
       <c r="B35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="28">
         <v>0.11082599999999999</v>
       </c>
-      <c r="D35" s="27"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="13">
         <v>2.0470000000000002</v>
       </c>
@@ -3189,10 +3265,10 @@
       <c r="G35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H35" s="26">
+      <c r="H35" s="28">
         <v>-1.8029999999999999</v>
       </c>
-      <c r="I35" s="27"/>
+      <c r="I35" s="29"/>
       <c r="J35" s="14">
         <v>-1.502</v>
       </c>
@@ -3202,17 +3278,17 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="27"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="28">
+      <c r="H36" s="32">
         <v>0.34889999999999999</v>
       </c>
-      <c r="I36" s="29"/>
+      <c r="I36" s="33"/>
       <c r="J36" s="13">
         <v>2.6030000000000002</v>
       </c>
@@ -3224,10 +3300,10 @@
       <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="28">
         <v>4.2290000000000001E-3</v>
       </c>
-      <c r="D37" s="27"/>
+      <c r="D37" s="29"/>
       <c r="E37" s="14">
         <v>1.752</v>
       </c>
@@ -3237,10 +3313,10 @@
       <c r="G37" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H37" s="28">
+      <c r="H37" s="32">
         <v>0.17349999999999999</v>
       </c>
-      <c r="I37" s="29"/>
+      <c r="I37" s="33"/>
       <c r="J37" s="13">
         <v>2.0430000000000001</v>
       </c>
@@ -3250,17 +3326,17 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="3"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="28">
+      <c r="H38" s="32">
         <v>0.62290000000000001</v>
       </c>
-      <c r="I38" s="29"/>
+      <c r="I38" s="33"/>
       <c r="J38" s="13">
         <v>2.3220000000000001</v>
       </c>
@@ -3270,17 +3346,17 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="28">
+      <c r="H39" s="32">
         <v>3.5459999999999998E-2</v>
       </c>
-      <c r="I39" s="29"/>
+      <c r="I39" s="33"/>
       <c r="J39" s="14">
         <v>1.673</v>
       </c>
@@ -3290,17 +3366,17 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="28">
+      <c r="H40" s="32">
         <v>0.12790000000000001</v>
       </c>
-      <c r="I40" s="29"/>
+      <c r="I40" s="33"/>
       <c r="J40" s="14">
         <v>1.909</v>
       </c>
@@ -3312,10 +3388,10 @@
       <c r="B41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="28">
         <v>-3.9529999999999999E-3</v>
       </c>
-      <c r="D41" s="27"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="13">
         <v>-1.9850000000000001</v>
       </c>
@@ -3325,10 +3401,10 @@
       <c r="G41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="28">
+      <c r="H41" s="32">
         <v>6.275E-2</v>
       </c>
-      <c r="I41" s="29"/>
+      <c r="I41" s="33"/>
       <c r="J41" s="14">
         <v>1.4390000000000001</v>
       </c>
@@ -3338,17 +3414,17 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="3"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="G42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H42" s="28">
+      <c r="H42" s="32">
         <v>-1.226E-2</v>
       </c>
-      <c r="I42" s="29"/>
+      <c r="I42" s="33"/>
       <c r="J42" s="13">
         <v>-2.516</v>
       </c>
@@ -3358,17 +3434,17 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" s="3"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
       <c r="G43" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="28">
+      <c r="H43" s="32">
         <v>-2.5200000000000001E-3</v>
       </c>
-      <c r="I43" s="29"/>
+      <c r="I43" s="33"/>
       <c r="J43" s="13">
         <v>-2.129</v>
       </c>
@@ -3378,17 +3454,17 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H44" s="28">
+      <c r="H44" s="32">
         <v>-1.235E-3</v>
       </c>
-      <c r="I44" s="29"/>
+      <c r="I44" s="33"/>
       <c r="J44" s="14">
         <v>-1.601</v>
       </c>
@@ -3398,17 +3474,17 @@
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" s="3"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
       <c r="G45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="28">
+      <c r="H45" s="32">
         <v>-4.4869999999999997E-3</v>
       </c>
-      <c r="I45" s="29"/>
+      <c r="I45" s="33"/>
       <c r="J45" s="14">
         <v>-1.8380000000000001</v>
       </c>
@@ -3418,17 +3494,17 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" s="3"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
       <c r="G46" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H46" s="28">
+      <c r="H46" s="32">
         <v>8.8200000000000003E-5</v>
       </c>
-      <c r="I46" s="29"/>
+      <c r="I46" s="33"/>
       <c r="J46" s="13">
         <v>2.0419999999999998</v>
       </c>
@@ -3554,10 +3630,10 @@
       <c r="B55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="26">
+      <c r="C55" s="28">
         <v>6656.6639999999998</v>
       </c>
-      <c r="D55" s="27"/>
+      <c r="D55" s="29"/>
       <c r="E55" s="14">
         <v>1.9119999999999999</v>
       </c>
@@ -3567,10 +3643,10 @@
       <c r="G55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H55" s="26">
+      <c r="H55" s="28">
         <v>1673.6934000000001</v>
       </c>
-      <c r="I55" s="27"/>
+      <c r="I55" s="29"/>
       <c r="J55" s="14">
         <v>2.2320000000000002</v>
       </c>
@@ -3580,17 +3656,17 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" s="3"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="27"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="29"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H56" s="26">
+      <c r="H56" s="28">
         <v>-34.612099999999998</v>
       </c>
-      <c r="I56" s="27"/>
+      <c r="I56" s="29"/>
       <c r="J56" s="14">
         <v>-2.4380000000000002</v>
       </c>
@@ -3602,10 +3678,10 @@
       <c r="B57" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="26">
+      <c r="C57" s="28">
         <v>-423.01299999999998</v>
       </c>
-      <c r="D57" s="27"/>
+      <c r="D57" s="29"/>
       <c r="E57" s="13">
         <v>-2.1219999999999999</v>
       </c>
@@ -3613,8 +3689,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="27"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="29"/>
       <c r="J57" s="14"/>
       <c r="K57" s="14"/>
     </row>
@@ -3622,10 +3698,10 @@
       <c r="B58" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="26">
+      <c r="C58" s="28">
         <v>-251.28800000000001</v>
       </c>
-      <c r="D58" s="27"/>
+      <c r="D58" s="29"/>
       <c r="E58" s="14">
         <v>-1.966</v>
       </c>
@@ -3633,24 +3709,24 @@
         <v>5.0599999999999999E-2</v>
       </c>
       <c r="G58" s="1"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="27"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="29"/>
       <c r="J58" s="14"/>
       <c r="K58" s="14"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" s="3"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="29"/>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H59" s="26">
+      <c r="H59" s="28">
         <v>-13.111700000000001</v>
       </c>
-      <c r="I59" s="27"/>
+      <c r="I59" s="29"/>
       <c r="J59" s="14">
         <v>-1.8180000000000001</v>
       </c>
@@ -3662,10 +3738,10 @@
       <c r="B60" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="26">
+      <c r="C60" s="28">
         <v>16.175000000000001</v>
       </c>
-      <c r="D60" s="27"/>
+      <c r="D60" s="29"/>
       <c r="E60" s="13">
         <v>2.2109999999999999</v>
       </c>
@@ -3673,24 +3749,24 @@
         <v>2.81E-2</v>
       </c>
       <c r="G60" s="1"/>
-      <c r="H60" s="26"/>
-      <c r="I60" s="27"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="29"/>
       <c r="J60" s="14"/>
       <c r="K60" s="14"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
       <c r="G61" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H61" s="26">
+      <c r="H61" s="28">
         <v>0.28439999999999999</v>
       </c>
-      <c r="I61" s="27"/>
+      <c r="I61" s="29"/>
       <c r="J61" s="14">
         <v>2.1880000000000002</v>
       </c>
@@ -3700,18 +3776,71 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="G51:K51"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="H59:I59"/>
     <mergeCell ref="C60:D60"/>
@@ -3728,71 +3857,18 @@
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="C54:D54"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="G51:K51"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3832,10 +3908,10 @@
         <v>22</v>
       </c>
       <c r="C3" s="30"/>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -3955,10 +4031,10 @@
         <v>65</v>
       </c>
       <c r="C19" s="30"/>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="37"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
@@ -4169,10 +4245,10 @@
         <v>22</v>
       </c>
       <c r="C38" s="30"/>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="37"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
@@ -4304,15 +4380,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>